<commit_message>
Nouveau logo + Changement PACMAC en PACMAN
</commit_message>
<xml_diff>
--- a/CaractereBinHex.xlsx
+++ b/CaractereBinHex.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastien\CloudStation\HEIG\3eme\APM\PacMan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastien\CloudStation\HEIG\3eme\APM\PacMan\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CaractereBinHex" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>CORNER_TOP_LEFT</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>PACMAC_NO_MOVE</t>
+  </si>
+  <si>
+    <t>PACMAC_EAT</t>
+  </si>
+  <si>
+    <t>GHOST</t>
+  </si>
+  <si>
+    <t>COIN</t>
+  </si>
+  <si>
+    <t>PACMAC_DEAD</t>
   </si>
 </sst>
 </file>
@@ -878,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -893,91 +905,91 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CharactereBinHex!L3</f>
-        <v>00 7E 7E 60 60 60 60 00</v>
+        <v>00 7F 7F 60 60 60 60 60</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CharactereBinHex!L13</f>
-        <v>00 60 60 60 60 7E 7E 00</v>
+        <v>60 60 60 60 60 7F 7F 00</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CharactereBinHex!L23</f>
-        <v>00 7E 7E 06 06 06 06 00</v>
+        <v>00 FE FE 06 06 06 06 06</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CharactereBinHex!L33</f>
-        <v>00 06 06 06 06 7E 7E 00</v>
+        <v>06 06 06 06 06 FE FE 00</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CharactereBinHex!L43</f>
-        <v>00 7E 7E 18 18 18 18 00</v>
+        <v>00 FF FF 18 18 18 18 18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>CharactereBinHex!L53</f>
-        <v>00 18 18 18 18 1E 7E 00</v>
+        <v>00 18 18 18 18 FF FF 00</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>CharactereBinHex!L63</f>
-        <v>00 60 60 7E 7E 60 60 00</v>
+        <v>60 60 60 7F 7F 60 60 60</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CharactereBinHex!L73</f>
-        <v>00 06 06 7E 7E 06 06 00</v>
+        <v>06 06 06 FE FE 06 06 06</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>CharactereBinHex!L83</f>
-        <v>00 7E 7E 00 00 00 00 00</v>
+        <v>00 FF FF 00 00 00 00 00</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CharactereBinHex!L93</f>
-        <v>00 00 00 7E 7E 00 00 00</v>
+        <v>00 00 00 FF FF 00 00 00</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CharactereBinHex!L103</f>
-        <v>00 00 00 00 00 7E 7E 00</v>
+        <v>00 00 00 00 00 FF FF 00</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CharactereBinHex!L113</f>
-        <v>00 60 60 60 60 60 60 00</v>
+        <v>60 60 60 60 60 60 60 60</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CharactereBinHex!L123</f>
-        <v>00 18 18 18 18 18 18 00</v>
+        <v>18 18 18 18 18 18 18 18</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>CharactereBinHex!L133</f>
-        <v>00 06 06 06 06 06 06 00</v>
+        <v>06 06 06 06 06 06 06 06</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>CharactereBinHex!L143</f>
-        <v>00 3C 6E 78 78 7E 3C 00</v>
+        <v>00 3C 7E 78 78 7E 3C 00</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -989,19 +1001,37 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>CharactereBinHex!L163</f>
-        <v>00 24 66 7E 5E 7E 3C 00</v>
+        <v>00 24 66 7E 7E 7E 3C 00</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>CharactereBinHex!L173</f>
-        <v>00 3C 76 1E 1E 7E 3C 00</v>
+        <v>00 3C 7E 1E 1E 7E 3C 00</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>CharactereBinHex!L183</f>
-        <v>00 3C 7E 5E 7E 66 24 00</v>
+        <v>00 3C 7E 7E 7E 66 24 00</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>CharactereBinHex!L193</f>
+        <v>00 3C 7E 7E 7E 7E 3C 00</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>CharactereBinHex!L203</f>
+        <v>00 3C 5A 66 66 5A 3C 00</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>CharactereBinHex!L212</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1011,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L190"/>
+  <dimension ref="A1:L230"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="L223" sqref="L223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1110,7 @@
       </c>
       <c r="L3" t="str">
         <f xml:space="preserve"> K3 &amp; " " &amp; K4 &amp; " " &amp; K5 &amp; " " &amp; K6 &amp; " " &amp; K7 &amp; " " &amp; K8 &amp; " " &amp; K9 &amp; " " &amp; K10</f>
-        <v>00 7E 7E 60 60 60 60 00</v>
+        <v>00 7F 7F 60 60 60 60 60</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1106,11 +1136,11 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1" t="str">
         <f t="shared" ref="K4:K10" si="0" xml:space="preserve"> DEC2HEX(IF(A4=1,128,0) + IF(B4=1,64,0)+IF(C4=1,32,0)+IF(D4=1,16,0)+IF(E4=1,8,0)+IF(F4=1,4,0)+IF(G4=1,2,0)+IF(H4=1,1,0),2)</f>
-        <v>7E</v>
+        <v>7F</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1136,11 +1166,11 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>7E</v>
+        <v>7F</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1268,10 +1298,10 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1290,7 +1320,7 @@
       </c>
       <c r="K10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1317,10 +1347,10 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1339,11 +1369,11 @@
       </c>
       <c r="K13" s="1" t="str">
         <f xml:space="preserve"> DEC2HEX(IF(A13=1,128,0) + IF(B13=1,64,0)+IF(C13=1,32,0)+IF(D13=1,16,0)+IF(E13=1,8,0)+IF(F13=1,4,0)+IF(G13=1,2,0)+IF(H13=1,1,0),2)</f>
-        <v>00</v>
+        <v>60</v>
       </c>
       <c r="L13" t="str">
         <f xml:space="preserve"> K13 &amp; " " &amp; K14 &amp; " " &amp; K15 &amp; " " &amp; K16 &amp; " " &amp; K17 &amp; " " &amp; K18 &amp; " " &amp; K19 &amp; " " &amp; K20</f>
-        <v>00 60 60 60 60 7E 7E 00</v>
+        <v>60 60 60 60 60 7F 7F 00</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1489,11 +1519,11 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>7E</v>
+        <v>7F</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1519,11 +1549,11 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>7E</v>
+        <v>7F</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1603,12 +1633,12 @@
       </c>
       <c r="L23" t="str">
         <f xml:space="preserve"> K23 &amp; " " &amp; K24 &amp; " " &amp; K25 &amp; " " &amp; K26 &amp; " " &amp; K27 &amp; " " &amp; K28 &amp; " " &amp; K29 &amp; " " &amp; K30</f>
-        <v>00 7E 7E 06 06 06 06 00</v>
+        <v>00 FE FE 06 06 06 06 06</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1633,12 +1663,12 @@
       </c>
       <c r="K24" s="1" t="str">
         <f t="shared" ref="K24:K30" si="2" xml:space="preserve"> DEC2HEX(IF(A24=1,128,0) + IF(B24=1,64,0)+IF(C24=1,32,0)+IF(D24=1,16,0)+IF(E24=1,8,0)+IF(F24=1,4,0)+IF(G24=1,2,0)+IF(H24=1,1,0),2)</f>
-        <v>7E</v>
+        <v>FE</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1663,7 +1693,7 @@
       </c>
       <c r="K25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>7E</v>
+        <v>FE</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1803,17 +1833,17 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="K30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>00</v>
+        <v>06</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1849,21 +1879,21 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="K33" s="1" t="str">
         <f xml:space="preserve"> DEC2HEX(IF(A33=1,128,0) + IF(B33=1,64,0)+IF(C33=1,32,0)+IF(D33=1,16,0)+IF(E33=1,8,0)+IF(F33=1,4,0)+IF(G33=1,2,0)+IF(H33=1,1,0),2)</f>
-        <v>00</v>
+        <v>06</v>
       </c>
       <c r="L33" t="str">
         <f xml:space="preserve"> K33 &amp; " " &amp; K34 &amp; " " &amp; K35 &amp; " " &amp; K36 &amp; " " &amp; K37 &amp; " " &amp; K38 &amp; " " &amp; K39 &amp; " " &amp; K40</f>
-        <v>00 06 06 06 06 7E 7E 00</v>
+        <v>06 06 06 06 06 FE FE 00</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1988,7 +2018,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2013,12 +2043,12 @@
       </c>
       <c r="K38" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>7E</v>
+        <v>FE</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2043,7 +2073,7 @@
       </c>
       <c r="K39" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>7E</v>
+        <v>FE</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2126,12 +2156,12 @@
       </c>
       <c r="L43" t="str">
         <f xml:space="preserve"> K43 &amp; " " &amp; K44 &amp; " " &amp; K45 &amp; " " &amp; K46 &amp; " " &amp; K47 &amp; " " &amp; K48 &amp; " " &amp; K49 &amp; " " &amp; K50</f>
-        <v>00 7E 7E 18 18 18 18 00</v>
+        <v>00 FF FF 18 18 18 18 18</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2152,16 +2182,16 @@
         <v>1</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="1" t="str">
         <f t="shared" ref="K44:K50" si="4" xml:space="preserve"> DEC2HEX(IF(A44=1,128,0) + IF(B44=1,64,0)+IF(C44=1,32,0)+IF(D44=1,16,0)+IF(E44=1,8,0)+IF(F44=1,4,0)+IF(G44=1,2,0)+IF(H44=1,1,0),2)</f>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2182,11 +2212,11 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2320,10 +2350,10 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -2336,7 +2366,7 @@
       </c>
       <c r="K50" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2389,7 +2419,7 @@
       </c>
       <c r="L53" t="str">
         <f xml:space="preserve"> K53 &amp; " " &amp; K54 &amp; " " &amp; K55 &amp; " " &amp; K56 &amp; " " &amp; K57 &amp; " " &amp; K58 &amp; " " &amp; K59 &amp; " " &amp; K60</f>
-        <v>00 18 18 18 18 1E 7E 00</v>
+        <v>00 18 18 18 18 FF FF 00</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -2514,13 +2544,13 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -2535,16 +2565,16 @@
         <v>1</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2565,11 +2595,11 @@
         <v>1</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -2623,10 +2653,10 @@
         <v>0</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2645,11 +2675,11 @@
       </c>
       <c r="K63" s="1" t="str">
         <f xml:space="preserve"> DEC2HEX(IF(A63=1,128,0) + IF(B63=1,64,0)+IF(C63=1,32,0)+IF(D63=1,16,0)+IF(E63=1,8,0)+IF(F63=1,4,0)+IF(G63=1,2,0)+IF(H63=1,1,0),2)</f>
-        <v>00</v>
+        <v>60</v>
       </c>
       <c r="L63" t="str">
         <f xml:space="preserve"> K63 &amp; " " &amp; K64 &amp; " " &amp; K65 &amp; " " &amp; K66 &amp; " " &amp; K67 &amp; " " &amp; K68 &amp; " " &amp; K69 &amp; " " &amp; K70</f>
-        <v>00 60 60 7E 7E 60 60 00</v>
+        <v>60 60 60 7F 7F 60 60 60</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -2735,11 +2765,11 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K66" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>7E</v>
+        <v>7F</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -2765,11 +2795,11 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K67" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>7E</v>
+        <v>7F</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -2837,10 +2867,10 @@
         <v>0</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -2859,7 +2889,7 @@
       </c>
       <c r="K70" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>00</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -2895,21 +2925,21 @@
         <v>0</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73">
         <v>0</v>
       </c>
       <c r="K73" s="1" t="str">
         <f xml:space="preserve"> DEC2HEX(IF(A73=1,128,0) + IF(B73=1,64,0)+IF(C73=1,32,0)+IF(D73=1,16,0)+IF(E73=1,8,0)+IF(F73=1,4,0)+IF(G73=1,2,0)+IF(H73=1,1,0),2)</f>
-        <v>00</v>
+        <v>06</v>
       </c>
       <c r="L73" t="str">
         <f xml:space="preserve"> K73 &amp; " " &amp; K74 &amp; " " &amp; K75 &amp; " " &amp; K76 &amp; " " &amp; K77 &amp; " " &amp; K78 &amp; " " &amp; K79 &amp; " " &amp; K80</f>
-        <v>00 06 06 7E 7E 06 06 00</v>
+        <v>06 06 06 FE FE 06 06 06</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -2974,7 +3004,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2999,12 +3029,12 @@
       </c>
       <c r="K76" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>7E</v>
+        <v>FE</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -3029,7 +3059,7 @@
       </c>
       <c r="K77" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>7E</v>
+        <v>FE</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3109,17 +3139,17 @@
         <v>0</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80">
         <v>0</v>
       </c>
       <c r="K80" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>00</v>
+        <v>06</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -3169,12 +3199,12 @@
       </c>
       <c r="L83" t="str">
         <f xml:space="preserve"> K83 &amp; " " &amp; K84 &amp; " " &amp; K85 &amp; " " &amp; K86 &amp; " " &amp; K87 &amp; " " &amp; K88 &amp; " " &amp; K89 &amp; " " &amp; K90</f>
-        <v>00 7E 7E 00 00 00 00 00</v>
+        <v>00 FF FF 00 00 00 00 00</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -3195,16 +3225,16 @@
         <v>1</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K84" s="1" t="str">
         <f t="shared" ref="K84:K90" si="8" xml:space="preserve"> DEC2HEX(IF(A84=1,128,0) + IF(B84=1,64,0)+IF(C84=1,32,0)+IF(D84=1,16,0)+IF(E84=1,8,0)+IF(F84=1,4,0)+IF(G84=1,2,0)+IF(H84=1,1,0),2)</f>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -3225,11 +3255,11 @@
         <v>1</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K85" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -3432,7 +3462,7 @@
       </c>
       <c r="L93" t="str">
         <f xml:space="preserve"> K93 &amp; " " &amp; K94 &amp; " " &amp; K95 &amp; " " &amp; K96 &amp; " " &amp; K97 &amp; " " &amp; K98 &amp; " " &amp; K99 &amp; " " &amp; K100</f>
-        <v>00 00 00 7E 7E 00 00 00</v>
+        <v>00 00 00 FF FF 00 00 00</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -3497,7 +3527,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -3518,16 +3548,16 @@
         <v>1</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K96" s="1" t="str">
         <f t="shared" si="9"/>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -3548,11 +3578,11 @@
         <v>1</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K97" s="1" t="str">
         <f t="shared" si="9"/>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -3692,7 +3722,7 @@
       </c>
       <c r="L103" t="str">
         <f xml:space="preserve"> K103 &amp; " " &amp; K104 &amp; " " &amp; K105 &amp; " " &amp; K106 &amp; " " &amp; K107 &amp; " " &amp; K108 &amp; " " &amp; K109 &amp; " " &amp; K110</f>
-        <v>00 00 00 00 00 7E 7E 00</v>
+        <v>00 00 00 00 00 FF FF 00</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -3817,7 +3847,7 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -3838,16 +3868,16 @@
         <v>1</v>
       </c>
       <c r="H108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K108" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -3868,11 +3898,11 @@
         <v>1</v>
       </c>
       <c r="H109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K109" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>7E</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -3926,10 +3956,10 @@
         <v>0</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -3948,11 +3978,11 @@
       </c>
       <c r="K113" s="1" t="str">
         <f xml:space="preserve"> DEC2HEX(IF(A113=1,128,0) + IF(B113=1,64,0)+IF(C113=1,32,0)+IF(D113=1,16,0)+IF(E113=1,8,0)+IF(F113=1,4,0)+IF(G113=1,2,0)+IF(H113=1,1,0),2)</f>
-        <v>00</v>
+        <v>60</v>
       </c>
       <c r="L113" t="str">
         <f xml:space="preserve"> K113 &amp; " " &amp; K114 &amp; " " &amp; K115 &amp; " " &amp; K116 &amp; " " &amp; K117 &amp; " " &amp; K118 &amp; " " &amp; K119 &amp; " " &amp; K120</f>
-        <v>00 60 60 60 60 60 60 00</v>
+        <v>60 60 60 60 60 60 60 60</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
@@ -4140,10 +4170,10 @@
         <v>0</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -4162,7 +4192,7 @@
       </c>
       <c r="K120" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>00</v>
+        <v>60</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
@@ -4192,10 +4222,10 @@
         <v>0</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F123">
         <v>0</v>
@@ -4208,11 +4238,11 @@
       </c>
       <c r="K123" s="1" t="str">
         <f xml:space="preserve"> DEC2HEX(IF(A123=1,128,0) + IF(B123=1,64,0)+IF(C123=1,32,0)+IF(D123=1,16,0)+IF(E123=1,8,0)+IF(F123=1,4,0)+IF(G123=1,2,0)+IF(H123=1,1,0),2)</f>
-        <v>00</v>
+        <v>18</v>
       </c>
       <c r="L123" t="str">
         <f xml:space="preserve"> K123 &amp; " " &amp; K124 &amp; " " &amp; K125 &amp; " " &amp; K126 &amp; " " &amp; K127 &amp; " " &amp; K128 &amp; " " &amp; K129 &amp; " " &amp; K130</f>
-        <v>00 18 18 18 18 18 18 00</v>
+        <v>18 18 18 18 18 18 18 18</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
@@ -4406,10 +4436,10 @@
         <v>0</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F130">
         <v>0</v>
@@ -4422,7 +4452,7 @@
       </c>
       <c r="K130" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>00</v>
+        <v>18</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
@@ -4458,21 +4488,21 @@
         <v>0</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H133">
         <v>0</v>
       </c>
       <c r="K133" s="1" t="str">
         <f xml:space="preserve"> DEC2HEX(IF(A133=1,128,0) + IF(B133=1,64,0)+IF(C133=1,32,0)+IF(D133=1,16,0)+IF(E133=1,8,0)+IF(F133=1,4,0)+IF(G133=1,2,0)+IF(H133=1,1,0),2)</f>
-        <v>00</v>
+        <v>06</v>
       </c>
       <c r="L133" t="str">
         <f xml:space="preserve"> K133 &amp; " " &amp; K134 &amp; " " &amp; K135 &amp; " " &amp; K136 &amp; " " &amp; K137 &amp; " " &amp; K138 &amp; " " &amp; K139 &amp; " " &amp; K140</f>
-        <v>00 06 06 06 06 06 06 00</v>
+        <v>06 06 06 06 06 06 06 06</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
@@ -4672,17 +4702,17 @@
         <v>0</v>
       </c>
       <c r="F140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H140">
         <v>0</v>
       </c>
       <c r="K140" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>00</v>
+        <v>06</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
@@ -4732,7 +4762,7 @@
       </c>
       <c r="L143" t="str">
         <f xml:space="preserve"> K143 &amp; " " &amp; K144 &amp; " " &amp; K145 &amp; " " &amp; K146 &amp; " " &amp; K147 &amp; " " &amp; K148 &amp; " " &amp; K149 &amp; " " &amp; K150</f>
-        <v>00 3C 6E 78 78 7E 3C 00</v>
+        <v>00 3C 7E 78 78 7E 3C 00</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
@@ -4776,7 +4806,7 @@
         <v>1</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -4792,7 +4822,7 @@
       </c>
       <c r="K145" s="1" t="str">
         <f t="shared" si="14"/>
-        <v>6E</v>
+        <v>7E</v>
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
@@ -5255,7 +5285,7 @@
       </c>
       <c r="L163" t="str">
         <f xml:space="preserve"> K163 &amp; " " &amp; K164 &amp; " " &amp; K165 &amp; " " &amp; K166 &amp; " " &amp; K167 &amp; " " &amp; K168 &amp; " " &amp; K169 &amp; " " &amp; K170</f>
-        <v>00 24 66 7E 5E 7E 3C 00</v>
+        <v>00 24 66 7E 7E 7E 3C 00</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
@@ -5356,7 +5386,7 @@
         <v>1</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D167">
         <v>1</v>
@@ -5375,7 +5405,7 @@
       </c>
       <c r="K167" s="1" t="str">
         <f t="shared" si="16"/>
-        <v>5E</v>
+        <v>7E</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
@@ -5515,7 +5545,7 @@
       </c>
       <c r="L173" t="str">
         <f xml:space="preserve"> K173 &amp; " " &amp; K174 &amp; " " &amp; K175 &amp; " " &amp; K176 &amp; " " &amp; K177 &amp; " " &amp; K178 &amp; " " &amp; K179 &amp; " " &amp; K180</f>
-        <v>00 3C 76 1E 1E 7E 3C 00</v>
+        <v>00 3C 7E 1E 1E 7E 3C 00</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
@@ -5562,7 +5592,7 @@
         <v>1</v>
       </c>
       <c r="E175">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F175">
         <v>1</v>
@@ -5575,7 +5605,7 @@
       </c>
       <c r="K175" s="1" t="str">
         <f t="shared" si="17"/>
-        <v>76</v>
+        <v>7E</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
@@ -5775,7 +5805,7 @@
       </c>
       <c r="L183" t="str">
         <f xml:space="preserve"> K183 &amp; " " &amp; K184 &amp; " " &amp; K185 &amp; " " &amp; K186 &amp; " " &amp; K187 &amp; " " &amp; K188 &amp; " " &amp; K189 &amp; " " &amp; K190</f>
-        <v>00 3C 7E 5E 7E 66 24 00</v>
+        <v>00 3C 7E 7E 7E 66 24 00</v>
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.25">
@@ -5846,7 +5876,7 @@
         <v>1</v>
       </c>
       <c r="C186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D186">
         <v>1</v>
@@ -5865,7 +5895,7 @@
       </c>
       <c r="K186" s="1" t="str">
         <f t="shared" si="18"/>
-        <v>5E</v>
+        <v>7E</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.25">
@@ -5988,8 +6018,1060 @@
         <v>00</v>
       </c>
     </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B192" s="2"/>
+      <c r="C192" s="2"/>
+      <c r="D192" s="2"/>
+      <c r="E192" s="2"/>
+      <c r="F192" s="2"/>
+      <c r="G192" s="2"/>
+      <c r="H192" s="2"/>
+      <c r="I192" s="2"/>
+      <c r="J192" s="2"/>
+      <c r="K192" s="2"/>
+      <c r="L192" s="2"/>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>0</v>
+      </c>
+      <c r="B193">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>0</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="K193" s="1" t="str">
+        <f xml:space="preserve"> DEC2HEX(IF(A193=1,128,0) + IF(B193=1,64,0)+IF(C193=1,32,0)+IF(D193=1,16,0)+IF(E193=1,8,0)+IF(F193=1,4,0)+IF(G193=1,2,0)+IF(H193=1,1,0),2)</f>
+        <v>00</v>
+      </c>
+      <c r="L193" t="str">
+        <f xml:space="preserve"> K193 &amp; " " &amp; K194 &amp; " " &amp; K195 &amp; " " &amp; K196 &amp; " " &amp; K197 &amp; " " &amp; K198 &amp; " " &amp; K199 &amp; " " &amp; K200</f>
+        <v>00 3C 7E 7E 7E 7E 3C 00</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>0</v>
+      </c>
+      <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+      <c r="E194">
+        <v>1</v>
+      </c>
+      <c r="F194">
+        <v>1</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
+      <c r="H194">
+        <v>0</v>
+      </c>
+      <c r="K194" s="1" t="str">
+        <f t="shared" ref="K194:K200" si="19" xml:space="preserve"> DEC2HEX(IF(A194=1,128,0) + IF(B194=1,64,0)+IF(C194=1,32,0)+IF(D194=1,16,0)+IF(E194=1,8,0)+IF(F194=1,4,0)+IF(G194=1,2,0)+IF(H194=1,1,0),2)</f>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>0</v>
+      </c>
+      <c r="B195">
+        <v>1</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+      <c r="E195">
+        <v>1</v>
+      </c>
+      <c r="F195">
+        <v>1</v>
+      </c>
+      <c r="G195">
+        <v>1</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="K195" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>0</v>
+      </c>
+      <c r="B196">
+        <v>1</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+      <c r="E196">
+        <v>1</v>
+      </c>
+      <c r="F196">
+        <v>1</v>
+      </c>
+      <c r="G196">
+        <v>1</v>
+      </c>
+      <c r="H196">
+        <v>0</v>
+      </c>
+      <c r="K196" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>0</v>
+      </c>
+      <c r="B197">
+        <v>1</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
+      <c r="E197">
+        <v>1</v>
+      </c>
+      <c r="F197">
+        <v>1</v>
+      </c>
+      <c r="G197">
+        <v>1</v>
+      </c>
+      <c r="H197">
+        <v>0</v>
+      </c>
+      <c r="K197" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>0</v>
+      </c>
+      <c r="B198">
+        <v>1</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="D198">
+        <v>1</v>
+      </c>
+      <c r="E198">
+        <v>1</v>
+      </c>
+      <c r="F198">
+        <v>1</v>
+      </c>
+      <c r="G198">
+        <v>1</v>
+      </c>
+      <c r="H198">
+        <v>0</v>
+      </c>
+      <c r="K198" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>0</v>
+      </c>
+      <c r="B199">
+        <v>0</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+      <c r="E199">
+        <v>1</v>
+      </c>
+      <c r="F199">
+        <v>1</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>0</v>
+      </c>
+      <c r="K199" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>0</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <v>0</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>0</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+      <c r="G200">
+        <v>0</v>
+      </c>
+      <c r="H200">
+        <v>0</v>
+      </c>
+      <c r="K200" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B202" s="2"/>
+      <c r="C202" s="2"/>
+      <c r="D202" s="2"/>
+      <c r="E202" s="2"/>
+      <c r="F202" s="2"/>
+      <c r="G202" s="2"/>
+      <c r="H202" s="2"/>
+      <c r="I202" s="2"/>
+      <c r="J202" s="2"/>
+      <c r="K202" s="2"/>
+      <c r="L202" s="2"/>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>0</v>
+      </c>
+      <c r="B203">
+        <v>0</v>
+      </c>
+      <c r="C203">
+        <v>0</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203">
+        <v>0</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <v>0</v>
+      </c>
+      <c r="K203" s="1" t="str">
+        <f xml:space="preserve"> DEC2HEX(IF(A203=1,128,0) + IF(B203=1,64,0)+IF(C203=1,32,0)+IF(D203=1,16,0)+IF(E203=1,8,0)+IF(F203=1,4,0)+IF(G203=1,2,0)+IF(H203=1,1,0),2)</f>
+        <v>00</v>
+      </c>
+      <c r="L203" t="str">
+        <f xml:space="preserve"> K203 &amp; " " &amp; K204 &amp; " " &amp; K205 &amp; " " &amp; K206 &amp; " " &amp; K207 &amp; " " &amp; K208 &amp; " " &amp; K209 &amp; " " &amp; K210</f>
+        <v>00 3C 5A 66 66 5A 3C 00</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>0</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
+      <c r="E204">
+        <v>1</v>
+      </c>
+      <c r="F204">
+        <v>1</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>0</v>
+      </c>
+      <c r="K204" s="1" t="str">
+        <f t="shared" ref="K204:K210" si="20" xml:space="preserve"> DEC2HEX(IF(A204=1,128,0) + IF(B204=1,64,0)+IF(C204=1,32,0)+IF(D204=1,16,0)+IF(E204=1,8,0)+IF(F204=1,4,0)+IF(G204=1,2,0)+IF(H204=1,1,0),2)</f>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>0</v>
+      </c>
+      <c r="B205">
+        <v>1</v>
+      </c>
+      <c r="C205">
+        <v>0</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+      <c r="E205">
+        <v>1</v>
+      </c>
+      <c r="F205">
+        <v>0</v>
+      </c>
+      <c r="G205">
+        <v>1</v>
+      </c>
+      <c r="H205">
+        <v>0</v>
+      </c>
+      <c r="K205" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>0</v>
+      </c>
+      <c r="B206">
+        <v>1</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>0</v>
+      </c>
+      <c r="F206">
+        <v>1</v>
+      </c>
+      <c r="G206">
+        <v>1</v>
+      </c>
+      <c r="H206">
+        <v>0</v>
+      </c>
+      <c r="K206" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>0</v>
+      </c>
+      <c r="B207">
+        <v>1</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207">
+        <v>0</v>
+      </c>
+      <c r="F207">
+        <v>1</v>
+      </c>
+      <c r="G207">
+        <v>1</v>
+      </c>
+      <c r="H207">
+        <v>0</v>
+      </c>
+      <c r="K207" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>0</v>
+      </c>
+      <c r="B208">
+        <v>1</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+      <c r="D208">
+        <v>1</v>
+      </c>
+      <c r="E208">
+        <v>1</v>
+      </c>
+      <c r="F208">
+        <v>0</v>
+      </c>
+      <c r="G208">
+        <v>1</v>
+      </c>
+      <c r="H208">
+        <v>0</v>
+      </c>
+      <c r="K208" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>0</v>
+      </c>
+      <c r="B209">
+        <v>0</v>
+      </c>
+      <c r="C209">
+        <v>1</v>
+      </c>
+      <c r="D209">
+        <v>1</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+      <c r="F209">
+        <v>1</v>
+      </c>
+      <c r="G209">
+        <v>0</v>
+      </c>
+      <c r="H209">
+        <v>0</v>
+      </c>
+      <c r="K209" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>0</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>0</v>
+      </c>
+      <c r="F210">
+        <v>0</v>
+      </c>
+      <c r="G210">
+        <v>0</v>
+      </c>
+      <c r="H210">
+        <v>0</v>
+      </c>
+      <c r="K210" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
+      <c r="E212" s="2"/>
+      <c r="F212" s="2"/>
+      <c r="G212" s="2"/>
+      <c r="H212" s="2"/>
+      <c r="I212" s="2"/>
+      <c r="J212" s="2"/>
+      <c r="K212" s="2"/>
+      <c r="L212" s="2"/>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>0</v>
+      </c>
+      <c r="B213">
+        <v>0</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>0</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="G213">
+        <v>0</v>
+      </c>
+      <c r="H213">
+        <v>0</v>
+      </c>
+      <c r="K213" s="1" t="str">
+        <f xml:space="preserve"> DEC2HEX(IF(A213=1,128,0) + IF(B213=1,64,0)+IF(C213=1,32,0)+IF(D213=1,16,0)+IF(E213=1,8,0)+IF(F213=1,4,0)+IF(G213=1,2,0)+IF(H213=1,1,0),2)</f>
+        <v>00</v>
+      </c>
+      <c r="L213" t="str">
+        <f xml:space="preserve"> K213 &amp; " " &amp; K214 &amp; " " &amp; K215 &amp; " " &amp; K216 &amp; " " &amp; K217 &amp; " " &amp; K218 &amp; " " &amp; K219 &amp; " " &amp; K220</f>
+        <v>00 3C 5A 7E 7E 5A 5A 00</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>0</v>
+      </c>
+      <c r="B214">
+        <v>0</v>
+      </c>
+      <c r="C214">
+        <v>1</v>
+      </c>
+      <c r="D214">
+        <v>1</v>
+      </c>
+      <c r="E214">
+        <v>1</v>
+      </c>
+      <c r="F214">
+        <v>1</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
+      <c r="H214">
+        <v>0</v>
+      </c>
+      <c r="K214" s="1" t="str">
+        <f t="shared" ref="K214:K226" si="21" xml:space="preserve"> DEC2HEX(IF(A214=1,128,0) + IF(B214=1,64,0)+IF(C214=1,32,0)+IF(D214=1,16,0)+IF(E214=1,8,0)+IF(F214=1,4,0)+IF(G214=1,2,0)+IF(H214=1,1,0),2)</f>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>0</v>
+      </c>
+      <c r="B215">
+        <v>1</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+      <c r="D215">
+        <v>1</v>
+      </c>
+      <c r="E215">
+        <v>1</v>
+      </c>
+      <c r="F215">
+        <v>0</v>
+      </c>
+      <c r="G215">
+        <v>1</v>
+      </c>
+      <c r="H215">
+        <v>0</v>
+      </c>
+      <c r="K215" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>0</v>
+      </c>
+      <c r="B216">
+        <v>1</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+      <c r="D216">
+        <v>1</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+      <c r="F216">
+        <v>1</v>
+      </c>
+      <c r="G216">
+        <v>1</v>
+      </c>
+      <c r="H216">
+        <v>0</v>
+      </c>
+      <c r="K216" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>0</v>
+      </c>
+      <c r="B217">
+        <v>1</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+      <c r="D217">
+        <v>1</v>
+      </c>
+      <c r="E217">
+        <v>1</v>
+      </c>
+      <c r="F217">
+        <v>1</v>
+      </c>
+      <c r="G217">
+        <v>1</v>
+      </c>
+      <c r="H217">
+        <v>0</v>
+      </c>
+      <c r="K217" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>0</v>
+      </c>
+      <c r="B218">
+        <v>1</v>
+      </c>
+      <c r="C218">
+        <v>0</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+      <c r="F218">
+        <v>0</v>
+      </c>
+      <c r="G218">
+        <v>1</v>
+      </c>
+      <c r="H218">
+        <v>0</v>
+      </c>
+      <c r="K218" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>0</v>
+      </c>
+      <c r="B219">
+        <v>1</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+      <c r="E219">
+        <v>1</v>
+      </c>
+      <c r="F219">
+        <v>0</v>
+      </c>
+      <c r="G219">
+        <v>1</v>
+      </c>
+      <c r="H219">
+        <v>0</v>
+      </c>
+      <c r="K219" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>0</v>
+      </c>
+      <c r="B220">
+        <v>0</v>
+      </c>
+      <c r="C220">
+        <v>0</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>0</v>
+      </c>
+      <c r="F220">
+        <v>0</v>
+      </c>
+      <c r="G220">
+        <v>0</v>
+      </c>
+      <c r="H220">
+        <v>0</v>
+      </c>
+      <c r="K220" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B222" s="2"/>
+      <c r="C222" s="2"/>
+      <c r="D222" s="2"/>
+      <c r="E222" s="2"/>
+      <c r="F222" s="2"/>
+      <c r="G222" s="2"/>
+      <c r="H222" s="2"/>
+      <c r="I222" s="2"/>
+      <c r="J222" s="2"/>
+      <c r="K222" s="2"/>
+      <c r="L222" s="2"/>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>0</v>
+      </c>
+      <c r="B223">
+        <v>0</v>
+      </c>
+      <c r="C223">
+        <v>0</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>0</v>
+      </c>
+      <c r="F223">
+        <v>0</v>
+      </c>
+      <c r="G223">
+        <v>0</v>
+      </c>
+      <c r="H223">
+        <v>0</v>
+      </c>
+      <c r="K223" s="1" t="str">
+        <f xml:space="preserve"> DEC2HEX(IF(A223=1,128,0) + IF(B223=1,64,0)+IF(C223=1,32,0)+IF(D223=1,16,0)+IF(E223=1,8,0)+IF(F223=1,4,0)+IF(G223=1,2,0)+IF(H223=1,1,0),2)</f>
+        <v>00</v>
+      </c>
+      <c r="L223" t="str">
+        <f xml:space="preserve"> K223 &amp; " " &amp; K224 &amp; " " &amp; K225 &amp; " " &amp; K226 &amp; " " &amp; K227 &amp; " " &amp; K228 &amp; " " &amp; K229 &amp; " " &amp; K230</f>
+        <v>00 00 18 3C 3C 18 00 00</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>0</v>
+      </c>
+      <c r="B224">
+        <v>0</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>0</v>
+      </c>
+      <c r="F224">
+        <v>0</v>
+      </c>
+      <c r="G224">
+        <v>0</v>
+      </c>
+      <c r="H224">
+        <v>0</v>
+      </c>
+      <c r="K224" s="1" t="str">
+        <f t="shared" ref="K224:K230" si="22" xml:space="preserve"> DEC2HEX(IF(A224=1,128,0) + IF(B224=1,64,0)+IF(C224=1,32,0)+IF(D224=1,16,0)+IF(E224=1,8,0)+IF(F224=1,4,0)+IF(G224=1,2,0)+IF(H224=1,1,0),2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>0</v>
+      </c>
+      <c r="B225">
+        <v>0</v>
+      </c>
+      <c r="C225">
+        <v>0</v>
+      </c>
+      <c r="D225">
+        <v>1</v>
+      </c>
+      <c r="E225">
+        <v>1</v>
+      </c>
+      <c r="F225">
+        <v>0</v>
+      </c>
+      <c r="G225">
+        <v>0</v>
+      </c>
+      <c r="H225">
+        <v>0</v>
+      </c>
+      <c r="K225" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>0</v>
+      </c>
+      <c r="B226">
+        <v>0</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+      <c r="E226">
+        <v>1</v>
+      </c>
+      <c r="F226">
+        <v>1</v>
+      </c>
+      <c r="G226">
+        <v>0</v>
+      </c>
+      <c r="H226">
+        <v>0</v>
+      </c>
+      <c r="K226" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>0</v>
+      </c>
+      <c r="B227">
+        <v>0</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+      <c r="D227">
+        <v>1</v>
+      </c>
+      <c r="E227">
+        <v>1</v>
+      </c>
+      <c r="F227">
+        <v>1</v>
+      </c>
+      <c r="G227">
+        <v>0</v>
+      </c>
+      <c r="H227">
+        <v>0</v>
+      </c>
+      <c r="K227" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>0</v>
+      </c>
+      <c r="B228">
+        <v>0</v>
+      </c>
+      <c r="C228">
+        <v>0</v>
+      </c>
+      <c r="D228">
+        <v>1</v>
+      </c>
+      <c r="E228">
+        <v>1</v>
+      </c>
+      <c r="F228">
+        <v>0</v>
+      </c>
+      <c r="G228">
+        <v>0</v>
+      </c>
+      <c r="H228">
+        <v>0</v>
+      </c>
+      <c r="K228" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>0</v>
+      </c>
+      <c r="B229">
+        <v>0</v>
+      </c>
+      <c r="C229">
+        <v>0</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>0</v>
+      </c>
+      <c r="F229">
+        <v>0</v>
+      </c>
+      <c r="G229">
+        <v>0</v>
+      </c>
+      <c r="H229">
+        <v>0</v>
+      </c>
+      <c r="K229" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>0</v>
+      </c>
+      <c r="B230">
+        <v>0</v>
+      </c>
+      <c r="C230">
+        <v>0</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>0</v>
+      </c>
+      <c r="F230">
+        <v>0</v>
+      </c>
+      <c r="G230">
+        <v>0</v>
+      </c>
+      <c r="H230">
+        <v>0</v>
+      </c>
+      <c r="K230" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>00</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="24">
+    <mergeCell ref="A72:L72"/>
+    <mergeCell ref="A222:L222"/>
+    <mergeCell ref="A212:L212"/>
+    <mergeCell ref="A92:L92"/>
+    <mergeCell ref="A122:L122"/>
+    <mergeCell ref="A142:L142"/>
+    <mergeCell ref="A152:L152"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A32:L32"/>
+    <mergeCell ref="A22:L22"/>
     <mergeCell ref="A82:L82"/>
     <mergeCell ref="A102:L102"/>
     <mergeCell ref="A112:L112"/>
@@ -5997,19 +7079,11 @@
     <mergeCell ref="A42:L42"/>
     <mergeCell ref="A52:L52"/>
     <mergeCell ref="A62:L62"/>
-    <mergeCell ref="A72:L72"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A192:L192"/>
+    <mergeCell ref="A202:L202"/>
     <mergeCell ref="A162:L162"/>
     <mergeCell ref="A172:L172"/>
     <mergeCell ref="A182:L182"/>
-    <mergeCell ref="A92:L92"/>
-    <mergeCell ref="A122:L122"/>
-    <mergeCell ref="A142:L142"/>
-    <mergeCell ref="A152:L152"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mise à jour des caractère
</commit_message>
<xml_diff>
--- a/CaractereBinHex.xlsx
+++ b/CaractereBinHex.xlsx
@@ -46,18 +46,6 @@
     <t>LINE_RIGHT_VERTICAL</t>
   </si>
   <si>
-    <t>PACMAC_GO_RIGHT</t>
-  </si>
-  <si>
-    <t>PACMAC_GO_UP</t>
-  </si>
-  <si>
-    <t>PACMAC_GO_LEFT</t>
-  </si>
-  <si>
-    <t>PACMAC_GO_DOWN</t>
-  </si>
-  <si>
     <t>LINE_CENTER_HORIZONTAL</t>
   </si>
   <si>
@@ -76,19 +64,31 @@
     <t>T_RIGHT_VERTICAL</t>
   </si>
   <si>
-    <t>PACMAC_NO_MOVE</t>
-  </si>
-  <si>
-    <t>PACMAC_EAT</t>
-  </si>
-  <si>
     <t>GHOST</t>
   </si>
   <si>
     <t>COIN</t>
   </si>
   <si>
-    <t>PACMAC_DEAD</t>
+    <t>PACMAN_GO_LEFT</t>
+  </si>
+  <si>
+    <t>PACMAN_GO_DOWN</t>
+  </si>
+  <si>
+    <t>PACMAN_GO_UP</t>
+  </si>
+  <si>
+    <t>PACMAN_NO_MOVE</t>
+  </si>
+  <si>
+    <t>PACMAN_GO_RIGHT</t>
+  </si>
+  <si>
+    <t>PACMAN_EAT</t>
+  </si>
+  <si>
+    <t>PACMAN_DEAD</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1029,9 +1029,9 @@
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f>CharactereBinHex!L212</f>
-        <v>0</v>
+      <c r="A22" t="str">
+        <f>CharactereBinHex!L213</f>
+        <v>00 3C 5A 7E 7E 5A 5A 00</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1044,7 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="L223" sqref="L223"/>
+      <selection activeCell="A202" sqref="A202:L202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4197,7 +4197,7 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -4717,7 +4717,7 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -4980,7 +4980,7 @@
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -5240,7 +5240,7 @@
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -5760,7 +5760,7 @@
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -6540,7 +6540,7 @@
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -6800,7 +6800,7 @@
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>

</xml_diff>